<commit_message>
Agregado grafico al excel
</commit_message>
<xml_diff>
--- a/Test Rendimiento.xlsx
+++ b/Test Rendimiento.xlsx
@@ -142,6 +142,1358 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Metodos/Grado Polinomio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarMSucesivas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1867</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7486</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>186359</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>753738</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarRecursiva</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5051</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>556495</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2931105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarRecursivaPar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarProgDinamica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarMejorada</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarPow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarHorne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$8:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>terminoK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>desarrolloCompleto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$10:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="193046672"/>
+        <c:axId val="193050592"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="193046672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="193050592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="193050592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="193046672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,13 +1812,27 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3">
+        <v>78</v>
+      </c>
       <c r="I2" s="3">
         <v>1867</v>
       </c>
@@ -484,13 +1850,27 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>47</v>
+      </c>
+      <c r="G3" s="3">
+        <v>94</v>
+      </c>
+      <c r="H3" s="3">
+        <v>187</v>
+      </c>
       <c r="I3" s="3">
         <v>5051</v>
       </c>
@@ -500,32 +1880,34 @@
       <c r="K3" s="3">
         <v>556495</v>
       </c>
-      <c r="L3" s="3"/>
+      <c r="L3" s="3">
+        <v>2931105</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
         <v>16</v>
@@ -536,7 +1918,9 @@
       <c r="K4" s="3">
         <v>48</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -637,5 +2021,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>